<commit_message>
Casi listo todo lo de knn, solo falta compute distances y describir las variables que se usaron para knn, parte de adrian
</commit_message>
<xml_diff>
--- a/Registro de KNN.xlsx
+++ b/Registro de KNN.xlsx
@@ -116,13 +116,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,7 +407,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,28 +476,28 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J7" si="0">SUM(B3:I3)</f>
@@ -504,7 +505,7 @@
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K13" si="1">SUM(B3:E3)/J3 * 100</f>
-        <v>60.869565217391312</v>
+        <v>65.217391304347828</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -512,28 +513,28 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
@@ -541,7 +542,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="1"/>
-        <v>47.826086956521742</v>
+        <v>56.521739130434781</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -555,10 +556,10 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -567,10 +568,10 @@
         <v>2</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
@@ -586,28 +587,28 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
@@ -615,7 +616,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>65.217391304347828</v>
+        <v>60.869565217391312</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -623,28 +624,28 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7">
         <v>2</v>
       </c>
       <c r="I7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
@@ -652,7 +653,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>65.217391304347828</v>
+        <v>60.869565217391312</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -660,7 +661,7 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -669,10 +670,10 @@
         <v>5</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -681,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="I8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J8">
         <f>SUM(B8:I8)</f>
@@ -697,7 +698,7 @@
         <v>18</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -706,10 +707,10 @@
         <v>5</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -718,7 +719,7 @@
         <v>2</v>
       </c>
       <c r="I9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J9">
         <f t="shared" ref="J9:J13" si="2">SUM(B9:I9)</f>
@@ -726,7 +727,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>60.869565217391312</v>
+        <v>65.217391304347828</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -734,28 +735,28 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
@@ -763,7 +764,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
-        <v>60.869565217391312</v>
+        <v>69.565217391304344</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -771,28 +772,28 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>3</v>
       </c>
       <c r="I11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
@@ -800,7 +801,7 @@
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>60.869565217391312</v>
+        <v>65.217391304347828</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -808,28 +809,28 @@
         <v>22</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J12">
         <f t="shared" si="2"/>
@@ -837,45 +838,11 @@
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>60.869565217391312</v>
+        <v>65.217391304347828</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>25</v>
-      </c>
-      <c r="B13">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>3</v>
-      </c>
-      <c r="I13">
-        <v>5</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="1"/>
-        <v>56.521739130434781</v>
-      </c>
+      <c r="A13" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -932,28 +899,28 @@
         <v>1</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
         <v>0</v>
       </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
       <c r="H17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J17">
         <f t="shared" ref="J17:J21" si="3">SUM(B17:I17)</f>
@@ -969,28 +936,28 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J18">
         <f t="shared" si="3"/>
@@ -998,7 +965,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="4"/>
-        <v>52.173913043478258</v>
+        <v>65.217391304347828</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1006,28 +973,28 @@
         <v>7</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D19">
         <v>5</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <v>2</v>
       </c>
       <c r="I19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J19">
         <f t="shared" si="3"/>
@@ -1035,7 +1002,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="4"/>
-        <v>47.826086956521742</v>
+        <v>65.217391304347828</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1043,28 +1010,28 @@
         <v>10</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J20">
         <f t="shared" si="3"/>
@@ -1072,7 +1039,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="4"/>
-        <v>60.869565217391312</v>
+        <v>73.91304347826086</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1083,25 +1050,25 @@
         <v>4</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21">
         <v>2</v>
       </c>
       <c r="G21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J21">
         <f t="shared" si="3"/>
@@ -1109,7 +1076,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="4"/>
-        <v>60.869565217391312</v>
+        <v>73.91304347826086</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1120,25 +1087,25 @@
         <v>4</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22">
         <v>2</v>
       </c>
       <c r="G22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J22">
         <f>SUM(B22:I22)</f>
@@ -1146,7 +1113,7 @@
       </c>
       <c r="K22">
         <f>SUM(B22:E22)/J22 * 100</f>
-        <v>47.826086956521742</v>
+        <v>69.565217391304344</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1157,25 +1124,25 @@
         <v>4</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23">
         <v>2</v>
       </c>
       <c r="G23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J23">
         <f t="shared" ref="J23:J27" si="5">SUM(B23:I23)</f>
@@ -1183,7 +1150,7 @@
       </c>
       <c r="K23">
         <f t="shared" ref="K23:K27" si="6">SUM(B23:E23)/J23 * 100</f>
-        <v>52.173913043478258</v>
+        <v>73.91304347826086</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1191,28 +1158,28 @@
         <v>20</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J24">
         <f t="shared" si="5"/>
@@ -1220,7 +1187,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="6"/>
-        <v>56.521739130434781</v>
+        <v>69.565217391304344</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1228,28 +1195,28 @@
         <v>21</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J25">
         <f t="shared" si="5"/>
@@ -1257,7 +1224,7 @@
       </c>
       <c r="K25">
         <f t="shared" si="6"/>
-        <v>56.521739130434781</v>
+        <v>69.565217391304344</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1268,25 +1235,25 @@
         <v>4</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F26">
         <v>2</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J26">
         <f t="shared" si="5"/>
@@ -1294,45 +1261,11 @@
       </c>
       <c r="K26">
         <f t="shared" si="6"/>
-        <v>52.173913043478258</v>
+        <v>73.91304347826086</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>25</v>
-      </c>
-      <c r="B27">
-        <v>4</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27">
-        <v>4</v>
-      </c>
-      <c r="E27">
-        <v>3</v>
-      </c>
-      <c r="F27">
-        <v>2</v>
-      </c>
-      <c r="G27">
-        <v>3</v>
-      </c>
-      <c r="H27">
-        <v>3</v>
-      </c>
-      <c r="I27">
-        <v>2</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="5"/>
-        <v>23</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="6"/>
-        <v>56.521739130434781</v>
-      </c>
+      <c r="A27" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>